<commit_message>
Change years from 2014 to 2015 in example.xlsx
</commit_message>
<xml_diff>
--- a/static/src/example.xlsx
+++ b/static/src/example.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="288" yWindow="96" windowWidth="9540" windowHeight="4512"/>
@@ -390,7 +390,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,7 +400,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
-        <v>41734.565300925926</v>
+        <v>42099.565300925926</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -411,7 +411,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>41734.153738425928</v>
+        <v>42099.153738425928</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -422,7 +422,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>41735.532534722224</v>
+        <v>42100.532534722224</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -433,7 +433,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>41737.374803240738</v>
+        <v>42102.374803240738</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -444,7 +444,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>41739.088194444441</v>
+        <v>42104.088194444441</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
@@ -455,7 +455,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>41739.757372685184</v>
+        <v>42104.757372685184</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>41739.111643518518</v>
+        <v>42104.111643518518</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>

</xml_diff>